<commit_message>
Add visa bulletin for 2017-2
</commit_message>
<xml_diff>
--- a/generator/2017_01.xlsx
+++ b/generator/2017_01.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="visa" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="39">
   <si>
     <t>Family-Sponsored</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -71,18 +71,6 @@
     <t>F4</t>
   </si>
   <si>
-    <t>1st</t>
-  </si>
-  <si>
-    <t>2nd</t>
-  </si>
-  <si>
-    <t>3rd</t>
-  </si>
-  <si>
-    <t>Other Workers</t>
-  </si>
-  <si>
     <t>EB3</t>
   </si>
   <si>
@@ -135,45 +123,6 @@
   </si>
   <si>
     <t>06/08/1993</t>
-  </si>
-  <si>
-    <t>Employ-</t>
-  </si>
-  <si>
-    <t>ment</t>
-  </si>
-  <si>
-    <t>based</t>
-  </si>
-  <si>
-    <t>All Charge-</t>
-  </si>
-  <si>
-    <t>ability </t>
-  </si>
-  <si>
-    <t>Areas Except</t>
-  </si>
-  <si>
-    <t>Those Listed</t>
-  </si>
-  <si>
-    <t>CHINA-</t>
-  </si>
-  <si>
-    <t>mainland </t>
-  </si>
-  <si>
-    <t>born</t>
-  </si>
-  <si>
-    <t>INDIA</t>
-  </si>
-  <si>
-    <t>MEXICO</t>
-  </si>
-  <si>
-    <t>PHILIPPINES</t>
   </si>
   <si>
     <t>10/15/2012</t>
@@ -198,11 +147,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
-    <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -225,92 +173,21 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF5E5E5E"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color rgb="FF5E5E5E"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="5">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFAAAAAA"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFAAAAAA"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFAAAAAA"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFAAAAAA"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFAAAAAA"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFAAAAAA"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFAAAAAA"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFAAAAAA"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFAAAAAA"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFAAAAAA"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFAAAAAA"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FFAAAAAA"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -320,7 +197,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -333,34 +210,7 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="15" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -668,7 +518,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -707,19 +557,19 @@
         <v>10</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -727,19 +577,19 @@
         <v>11</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -747,19 +597,19 @@
         <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -767,19 +617,19 @@
         <v>13</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -787,19 +637,19 @@
         <v>14</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -830,10 +680,10 @@
         <v>9</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>9</v>
@@ -841,49 +691,49 @@
       <c r="F8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="8"/>
+      <c r="G8" s="6"/>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="G9" s="8"/>
+        <v>37</v>
+      </c>
+      <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="G10" s="8"/>
+        <v>37</v>
+      </c>
+      <c r="G10" s="6"/>
     </row>
     <row r="11" spans="1:7">
       <c r="B11" s="5"/>
@@ -922,10 +772,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:F21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -937,289 +787,7 @@
     <col min="6" max="6" width="17.88671875" customWidth="1"/>
     <col min="7" max="7" width="9.21875" bestFit="1" customWidth="1"/>
   </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1">
-      <c r="A1" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="7">
-        <v>40186</v>
-      </c>
-      <c r="C1" s="7">
-        <v>40186</v>
-      </c>
-      <c r="D1" s="7">
-        <v>40186</v>
-      </c>
-      <c r="E1" s="7">
-        <v>34811</v>
-      </c>
-      <c r="F1" s="7">
-        <v>38626</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1">
-      <c r="A2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="7">
-        <v>42085</v>
-      </c>
-      <c r="C2" s="7">
-        <v>42085</v>
-      </c>
-      <c r="D2" s="7">
-        <v>42085</v>
-      </c>
-      <c r="E2" s="7">
-        <v>42071</v>
-      </c>
-      <c r="F2" s="7">
-        <v>42085</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1">
-      <c r="A3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="7">
-        <v>40337</v>
-      </c>
-      <c r="C3" s="7">
-        <v>40337</v>
-      </c>
-      <c r="D3" s="7">
-        <v>40337</v>
-      </c>
-      <c r="E3" s="7">
-        <v>34987</v>
-      </c>
-      <c r="F3" s="7">
-        <v>38815</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="15" thickBot="1">
-      <c r="A4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="7">
-        <v>38412</v>
-      </c>
-      <c r="C4" s="7">
-        <v>38412</v>
-      </c>
-      <c r="D4" s="7">
-        <v>38412</v>
-      </c>
-      <c r="E4" s="7">
-        <v>34683</v>
-      </c>
-      <c r="F4" s="7">
-        <v>34578</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15" thickBot="1">
-      <c r="A5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="7">
-        <v>38008</v>
-      </c>
-      <c r="C5" s="7">
-        <v>37947</v>
-      </c>
-      <c r="D5" s="7">
-        <v>37756</v>
-      </c>
-      <c r="E5" s="7">
-        <v>35565</v>
-      </c>
-      <c r="F5" s="7">
-        <v>34128</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1"/>
-    <row r="9" spans="1:7" ht="15" thickBot="1">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-    </row>
-    <row r="10" spans="1:7" ht="15" thickBot="1">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-    </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-    </row>
-    <row r="12" spans="1:7" ht="15" thickBot="1">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-    </row>
-    <row r="13" spans="1:7" ht="15" thickBot="1"/>
-    <row r="14" spans="1:7">
-      <c r="A14" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="F14" s="13" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-    </row>
-    <row r="17" spans="1:6" ht="15" thickBot="1">
-      <c r="A17" s="12"/>
-      <c r="B17" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="12"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-    </row>
-    <row r="18" spans="1:6" ht="15" thickBot="1">
-      <c r="A18" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="15" thickBot="1">
-      <c r="A19" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="7">
-        <v>41197</v>
-      </c>
-      <c r="D19" s="7">
-        <v>39553</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="15" thickBot="1">
-      <c r="A20" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" s="7">
-        <v>42583</v>
-      </c>
-      <c r="C20" s="7">
-        <v>41525</v>
-      </c>
-      <c r="D20" s="7">
-        <v>38426</v>
-      </c>
-      <c r="E20" s="7">
-        <v>42583</v>
-      </c>
-      <c r="F20" s="7">
-        <v>40746</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="21" thickBot="1">
-      <c r="A21" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B21" s="7">
-        <v>42583</v>
-      </c>
-      <c r="C21" s="7">
-        <v>38687</v>
-      </c>
-      <c r="D21" s="7">
-        <v>38426</v>
-      </c>
-      <c r="E21" s="7">
-        <v>42583</v>
-      </c>
-      <c r="F21" s="7">
-        <v>40746</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="D14:D17"/>
-    <mergeCell ref="E14:E17"/>
-    <mergeCell ref="F14:F17"/>
-  </mergeCells>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>